<commit_message>
test cases file fixes
</commit_message>
<xml_diff>
--- a/Final Project Part1/TEST CASE.xlsx
+++ b/Final Project Part1/TEST CASE.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\majdh\OneDrive\שולחן העבודה\Automation_bootcamp\Final Project Part1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99D3057C-4442-4CC2-8E64-872F03FDD9E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C771E8B-E93F-4157-A94D-22D70B77E75B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="10260" xr2:uid="{6DB08689-E348-4E0B-8AED-3F8E8057D764}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="800" uniqueCount="139">
   <si>
     <t>Name of the test case</t>
   </si>
@@ -145,13 +145,7 @@
 will appear</t>
   </si>
   <si>
-    <t xml:space="preserve">Book search while signed in </t>
-  </si>
-  <si>
     <t>Run sign in flow as mentioned in the first test case</t>
-  </si>
-  <si>
-    <t>valid email and password, book name</t>
   </si>
   <si>
     <t>Enter the book name in the search bar that
@@ -492,6 +486,15 @@
   </si>
   <si>
     <t>Cookies pop up will disappear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Book search </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> book name</t>
+  </si>
+  <si>
+    <t>book name</t>
   </si>
 </sst>
 </file>
@@ -939,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D84E9B10-6DEB-4A0D-98B6-D1464F09588B}">
   <dimension ref="A1:C414"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A361" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="C373" sqref="C373"/>
+    <sheetView tabSelected="1" topLeftCell="A247" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C133" sqref="C133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.65"/>
@@ -952,7 +955,7 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A1" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.65">
@@ -1118,7 +1121,7 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A30" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.65">
@@ -1284,7 +1287,7 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A60" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.65">
@@ -1292,7 +1295,7 @@
         <v>0</v>
       </c>
       <c r="B62" s="3" t="s">
-        <v>33</v>
+        <v>136</v>
       </c>
     </row>
     <row r="63" spans="1:3" ht="57" x14ac:dyDescent="0.65">
@@ -1300,7 +1303,7 @@
         <v>1</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.65">
@@ -1308,7 +1311,7 @@
         <v>2</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
     </row>
     <row r="65" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -1359,10 +1362,10 @@
         <v>1</v>
       </c>
       <c r="B72" s="6" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="73" spans="1:3" ht="57" x14ac:dyDescent="0.65">
@@ -1370,7 +1373,7 @@
         <v>2</v>
       </c>
       <c r="B73" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C73" s="3" t="s">
         <v>19</v>
@@ -1381,10 +1384,10 @@
         <v>3</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.65">
@@ -1392,10 +1395,10 @@
         <v>4</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -1403,10 +1406,10 @@
         <v>5</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C76" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.65">
@@ -1446,7 +1449,7 @@
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A91" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.65">
@@ -1454,7 +1457,7 @@
         <v>0</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="94" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -1462,7 +1465,7 @@
         <v>1</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.65">
@@ -1470,7 +1473,7 @@
         <v>2</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>35</v>
+        <v>137</v>
       </c>
     </row>
     <row r="96" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -1521,10 +1524,10 @@
         <v>1</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C103" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="104" spans="1:3" ht="57" x14ac:dyDescent="0.65">
@@ -1532,7 +1535,7 @@
         <v>2</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C104" s="3" t="s">
         <v>19</v>
@@ -1543,10 +1546,10 @@
         <v>3</v>
       </c>
       <c r="B105" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C105" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.65">
@@ -1554,10 +1557,10 @@
         <v>4</v>
       </c>
       <c r="B106" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C106" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="107" spans="1:3" ht="28.5" x14ac:dyDescent="0.65">
@@ -1565,10 +1568,10 @@
         <v>5</v>
       </c>
       <c r="B107" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="C107" s="8" t="s">
         <v>45</v>
-      </c>
-      <c r="C107" s="8" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.65">
@@ -1608,7 +1611,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A121" s="1" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.65">
@@ -1616,7 +1619,7 @@
         <v>0</v>
       </c>
       <c r="B123" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="124" spans="1:2" ht="28.5" x14ac:dyDescent="0.65">
@@ -1624,7 +1627,7 @@
         <v>1</v>
       </c>
       <c r="B124" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.65">
@@ -1632,7 +1635,7 @@
         <v>2</v>
       </c>
       <c r="B125" s="3" t="s">
-        <v>35</v>
+        <v>138</v>
       </c>
     </row>
     <row r="126" spans="1:2" ht="42.75" x14ac:dyDescent="0.65">
@@ -1683,10 +1686,10 @@
         <v>1</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>34</v>
+        <v>16</v>
       </c>
       <c r="C133" s="3" t="s">
-        <v>26</v>
+        <v>15</v>
       </c>
     </row>
     <row r="134" spans="1:3" ht="57" x14ac:dyDescent="0.65">
@@ -1694,7 +1697,7 @@
         <v>2</v>
       </c>
       <c r="B134" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C134" s="3" t="s">
         <v>19</v>
@@ -1705,10 +1708,10 @@
         <v>3</v>
       </c>
       <c r="B135" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C135" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.65">
@@ -1716,10 +1719,10 @@
         <v>4</v>
       </c>
       <c r="B136" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C136" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="137" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -1727,10 +1730,10 @@
         <v>5</v>
       </c>
       <c r="B137" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="C137" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="C137" s="8" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.65">
@@ -1770,7 +1773,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A152" s="1" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.65">
@@ -1778,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="B154" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="155" spans="1:2" ht="28.5" x14ac:dyDescent="0.65">
@@ -1786,7 +1789,7 @@
         <v>1</v>
       </c>
       <c r="B155" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.65">
@@ -1794,7 +1797,7 @@
         <v>2</v>
       </c>
       <c r="B156" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="42.75" x14ac:dyDescent="0.65">
@@ -1845,7 +1848,7 @@
         <v>1</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C164" s="3" t="s">
         <v>26</v>
@@ -1856,7 +1859,7 @@
         <v>2</v>
       </c>
       <c r="B165" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C165" s="3" t="s">
         <v>19</v>
@@ -1867,10 +1870,10 @@
         <v>3</v>
       </c>
       <c r="B166" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C166" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="167" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -1878,10 +1881,10 @@
         <v>4</v>
       </c>
       <c r="B167" s="8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C167" s="8" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="168" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -1889,10 +1892,10 @@
         <v>5</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C168" s="8" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="169" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -1900,10 +1903,10 @@
         <v>6</v>
       </c>
       <c r="B169" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C169" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.65">
@@ -1911,10 +1914,10 @@
         <v>7</v>
       </c>
       <c r="B170" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C170" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="171" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -1922,10 +1925,10 @@
         <v>8</v>
       </c>
       <c r="B171" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C171" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.65">
@@ -1944,7 +1947,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A181" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.65">
@@ -1952,7 +1955,7 @@
         <v>0</v>
       </c>
       <c r="B183" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="184" spans="1:2" ht="28.5" x14ac:dyDescent="0.65">
@@ -1960,7 +1963,7 @@
         <v>1</v>
       </c>
       <c r="B184" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.65">
@@ -2019,7 +2022,7 @@
         <v>1</v>
       </c>
       <c r="B194" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C194" s="3" t="s">
         <v>26</v>
@@ -2030,10 +2033,10 @@
         <v>2</v>
       </c>
       <c r="B195" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C195" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.65">
@@ -2041,10 +2044,10 @@
         <v>3</v>
       </c>
       <c r="B196" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C196" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
     </row>
     <row r="197" spans="1:3" ht="28.5" x14ac:dyDescent="0.65">
@@ -2052,10 +2055,10 @@
         <v>4</v>
       </c>
       <c r="B197" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C197" s="8" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="198" spans="1:3" ht="28.5" x14ac:dyDescent="0.65">
@@ -2063,10 +2066,10 @@
         <v>5</v>
       </c>
       <c r="B198" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C198" s="8" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.65">
@@ -2088,7 +2091,7 @@
         <v>8</v>
       </c>
       <c r="B201" s="8" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C201" s="3"/>
     </row>
@@ -2108,7 +2111,7 @@
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.65">
       <c r="A214" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.65">
@@ -2116,7 +2119,7 @@
         <v>0</v>
       </c>
       <c r="B216" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="217" spans="1:2" ht="42.75" x14ac:dyDescent="0.65">
@@ -2124,7 +2127,7 @@
         <v>1</v>
       </c>
       <c r="B217" s="8" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="218" spans="1:2" ht="28.5" x14ac:dyDescent="0.65">
@@ -2132,7 +2135,7 @@
         <v>2</v>
       </c>
       <c r="B218" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="219" spans="1:2" ht="42.75" x14ac:dyDescent="0.65">
@@ -2183,7 +2186,7 @@
         <v>1</v>
       </c>
       <c r="B226" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C226" s="3" t="s">
         <v>26</v>
@@ -2194,7 +2197,7 @@
         <v>2</v>
       </c>
       <c r="B227" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C227" s="3" t="s">
         <v>19</v>
@@ -2205,10 +2208,10 @@
         <v>3</v>
       </c>
       <c r="B228" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C228" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="229" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2216,10 +2219,10 @@
         <v>4</v>
       </c>
       <c r="B229" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C229" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="230" spans="1:3" x14ac:dyDescent="0.65">
@@ -2227,7 +2230,7 @@
         <v>5</v>
       </c>
       <c r="B230" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C230" s="8" t="s">
         <v>19</v>
@@ -2238,7 +2241,7 @@
         <v>6</v>
       </c>
       <c r="B231" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C231" s="3" t="s">
         <v>19</v>
@@ -2249,10 +2252,10 @@
         <v>7</v>
       </c>
       <c r="B232" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C232" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="233" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2260,10 +2263,10 @@
         <v>8</v>
       </c>
       <c r="B233" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C233" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="234" spans="1:3" x14ac:dyDescent="0.65">
@@ -2271,10 +2274,10 @@
         <v>9</v>
       </c>
       <c r="B234" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C234" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="235" spans="1:3" ht="71.25" x14ac:dyDescent="0.65">
@@ -2282,15 +2285,15 @@
         <v>10</v>
       </c>
       <c r="B235" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C235" s="8" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
     </row>
     <row r="244" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A244" s="1" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="245" spans="1:3" x14ac:dyDescent="0.65">
@@ -2298,7 +2301,7 @@
         <v>0</v>
       </c>
       <c r="B245" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="246" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2306,7 +2309,7 @@
         <v>1</v>
       </c>
       <c r="B246" s="8" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
     </row>
     <row r="247" spans="1:3" ht="28.5" x14ac:dyDescent="0.65">
@@ -2314,7 +2317,7 @@
         <v>2</v>
       </c>
       <c r="B247" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="248" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2365,7 +2368,7 @@
         <v>1</v>
       </c>
       <c r="B255" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C255" s="3" t="s">
         <v>26</v>
@@ -2376,7 +2379,7 @@
         <v>2</v>
       </c>
       <c r="B256" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C256" s="3" t="s">
         <v>19</v>
@@ -2387,10 +2390,10 @@
         <v>3</v>
       </c>
       <c r="B257" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C257" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="258" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2398,10 +2401,10 @@
         <v>4</v>
       </c>
       <c r="B258" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C258" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="259" spans="1:3" x14ac:dyDescent="0.65">
@@ -2409,7 +2412,7 @@
         <v>5</v>
       </c>
       <c r="B259" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C259" s="8" t="s">
         <v>19</v>
@@ -2420,7 +2423,7 @@
         <v>6</v>
       </c>
       <c r="B260" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C260" s="3" t="s">
         <v>19</v>
@@ -2431,10 +2434,10 @@
         <v>7</v>
       </c>
       <c r="B261" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C261" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="262" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2442,10 +2445,10 @@
         <v>8</v>
       </c>
       <c r="B262" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C262" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="263" spans="1:3" x14ac:dyDescent="0.65">
@@ -2453,10 +2456,10 @@
         <v>9</v>
       </c>
       <c r="B263" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C263" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="264" spans="1:3" ht="28.5" x14ac:dyDescent="0.65">
@@ -2464,10 +2467,10 @@
         <v>10</v>
       </c>
       <c r="B264" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C264" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="265" spans="1:3" x14ac:dyDescent="0.65">
@@ -2477,7 +2480,7 @@
     </row>
     <row r="274" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A274" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
     </row>
     <row r="275" spans="1:3" x14ac:dyDescent="0.65">
@@ -2485,7 +2488,7 @@
         <v>0</v>
       </c>
       <c r="B275" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
     </row>
     <row r="276" spans="1:3" ht="28.5" x14ac:dyDescent="0.65">
@@ -2493,7 +2496,7 @@
         <v>1</v>
       </c>
       <c r="B276" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="277" spans="1:3" ht="28.5" x14ac:dyDescent="0.65">
@@ -2501,7 +2504,7 @@
         <v>2</v>
       </c>
       <c r="B277" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="278" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2552,7 +2555,7 @@
         <v>1</v>
       </c>
       <c r="B285" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C285" s="3" t="s">
         <v>26</v>
@@ -2563,7 +2566,7 @@
         <v>2</v>
       </c>
       <c r="B286" s="8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C286" s="3" t="s">
         <v>19</v>
@@ -2574,10 +2577,10 @@
         <v>3</v>
       </c>
       <c r="B287" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C287" s="3" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="288" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2585,10 +2588,10 @@
         <v>4</v>
       </c>
       <c r="B288" s="8" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C288" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="289" spans="1:3" x14ac:dyDescent="0.65">
@@ -2596,7 +2599,7 @@
         <v>5</v>
       </c>
       <c r="B289" s="8" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C289" s="8" t="s">
         <v>19</v>
@@ -2607,7 +2610,7 @@
         <v>6</v>
       </c>
       <c r="B290" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C290" s="3" t="s">
         <v>19</v>
@@ -2618,10 +2621,10 @@
         <v>7</v>
       </c>
       <c r="B291" s="8" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C291" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="292" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2629,10 +2632,10 @@
         <v>8</v>
       </c>
       <c r="B292" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C292" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="293" spans="1:3" x14ac:dyDescent="0.65">
@@ -2640,10 +2643,10 @@
         <v>9</v>
       </c>
       <c r="B293" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C293" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
     </row>
     <row r="294" spans="1:3" x14ac:dyDescent="0.65">
@@ -2651,10 +2654,10 @@
         <v>10</v>
       </c>
       <c r="B294" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C294" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="295" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2662,10 +2665,10 @@
         <v>11</v>
       </c>
       <c r="B295" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C295" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="296" spans="1:3" ht="28.5" x14ac:dyDescent="0.65">
@@ -2673,10 +2676,10 @@
         <v>12</v>
       </c>
       <c r="B296" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C296" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="297" spans="1:3" ht="57" x14ac:dyDescent="0.65">
@@ -2684,15 +2687,15 @@
         <v>13</v>
       </c>
       <c r="B297" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C297" s="8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
     </row>
     <row r="304" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A304" s="1" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="306" spans="1:3" x14ac:dyDescent="0.65">
@@ -2700,7 +2703,7 @@
         <v>0</v>
       </c>
       <c r="B306" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="307" spans="1:3" x14ac:dyDescent="0.65">
@@ -2708,7 +2711,7 @@
         <v>1</v>
       </c>
       <c r="B307" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="308" spans="1:3" x14ac:dyDescent="0.65">
@@ -2716,7 +2719,7 @@
         <v>2</v>
       </c>
       <c r="B308" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="309" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2767,7 +2770,7 @@
         <v>1</v>
       </c>
       <c r="B316" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C316" s="3" t="s">
         <v>26</v>
@@ -2778,10 +2781,10 @@
         <v>2</v>
       </c>
       <c r="B317" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C317" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="318" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2789,7 +2792,7 @@
         <v>3</v>
       </c>
       <c r="B318" s="8" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C318" s="3" t="s">
         <v>19</v>
@@ -2800,10 +2803,10 @@
         <v>4</v>
       </c>
       <c r="B319" s="3" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C319" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="320" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2811,10 +2814,10 @@
         <v>5</v>
       </c>
       <c r="B320" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="C320" s="8" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="321" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2822,10 +2825,10 @@
         <v>6</v>
       </c>
       <c r="B321" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C321" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="322" spans="1:3" x14ac:dyDescent="0.65">
@@ -2833,10 +2836,10 @@
         <v>7</v>
       </c>
       <c r="B322" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C322" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="323" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2844,10 +2847,10 @@
         <v>8</v>
       </c>
       <c r="B323" s="8" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C323" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="324" spans="1:3" x14ac:dyDescent="0.65">
@@ -2866,7 +2869,7 @@
     </row>
     <row r="333" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A333" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="335" spans="1:3" x14ac:dyDescent="0.65">
@@ -2874,7 +2877,7 @@
         <v>0</v>
       </c>
       <c r="B335" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="336" spans="1:3" x14ac:dyDescent="0.65">
@@ -2882,7 +2885,7 @@
         <v>1</v>
       </c>
       <c r="B336" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="337" spans="1:3" x14ac:dyDescent="0.65">
@@ -2890,7 +2893,7 @@
         <v>2</v>
       </c>
       <c r="B337" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="338" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -2941,7 +2944,7 @@
         <v>1</v>
       </c>
       <c r="B345" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C345" s="3" t="s">
         <v>26</v>
@@ -2952,10 +2955,10 @@
         <v>2</v>
       </c>
       <c r="B346" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C346" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="347" spans="1:3" x14ac:dyDescent="0.65">
@@ -2963,10 +2966,10 @@
         <v>3</v>
       </c>
       <c r="B347" s="8" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C347" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="348" spans="1:3" x14ac:dyDescent="0.65">
@@ -2974,10 +2977,10 @@
         <v>4</v>
       </c>
       <c r="B348" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C348" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="349" spans="1:3" ht="28.5" x14ac:dyDescent="0.65">
@@ -2985,10 +2988,10 @@
         <v>5</v>
       </c>
       <c r="B349" s="8" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C349" s="8" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="350" spans="1:3" x14ac:dyDescent="0.65">
@@ -3028,7 +3031,7 @@
     </row>
     <row r="361" spans="1:3" x14ac:dyDescent="0.65">
       <c r="A361" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="363" spans="1:3" x14ac:dyDescent="0.65">
@@ -3036,7 +3039,7 @@
         <v>0</v>
       </c>
       <c r="B363" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="364" spans="1:3" x14ac:dyDescent="0.65">
@@ -3044,7 +3047,7 @@
         <v>1</v>
       </c>
       <c r="B364" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="365" spans="1:3" x14ac:dyDescent="0.65">
@@ -3052,7 +3055,7 @@
         <v>2</v>
       </c>
       <c r="B365" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="366" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -3103,10 +3106,10 @@
         <v>1</v>
       </c>
       <c r="B373" s="6" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C373" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="374" spans="1:3" ht="28.5" x14ac:dyDescent="0.65">
@@ -3114,10 +3117,10 @@
         <v>2</v>
       </c>
       <c r="B374" s="8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C374" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="375" spans="1:3" ht="42.75" x14ac:dyDescent="0.65">
@@ -3125,10 +3128,10 @@
         <v>3</v>
       </c>
       <c r="B375" s="8" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C375" s="8" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="376" spans="1:3" x14ac:dyDescent="0.65">

</xml_diff>